<commit_message>
import excel sheet update 2
</commit_message>
<xml_diff>
--- a/data/true and false question.xlsx
+++ b/data/true and false question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\graduation-project--master\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC928011-7826-4FC3-B98F-54117330E1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E6758A-3ABF-4CB4-A75C-695AD4626C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{60A39F5B-4EDB-4B9B-9637-46C26B568C21}"/>
   </bookViews>
@@ -34,40 +34,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>question</t>
   </si>
   <si>
-    <t>answer1</t>
-  </si>
-  <si>
-    <t>answer2</t>
-  </si>
-  <si>
     <t>correct_answer</t>
   </si>
   <si>
     <t>degree</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
-    <t>The Big Apple is a nickname given to Washington D.C in 1971.</t>
-  </si>
-  <si>
     <t>easy</t>
+  </si>
+  <si>
+    <t>frameborder attribute is not essential under &lt;iframe&gt;?</t>
+  </si>
+  <si>
+    <t>&lt;em&gt; works similar to &lt;b&gt; element?</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>&lt;u&gt; is used to underline the text in HTML?</t>
+  </si>
+  <si>
+    <t>difficult</t>
+  </si>
+  <si>
+    <t>&lt;frame&gt;  is used for YouTube videos?</t>
+  </si>
+  <si>
+    <t>&lt;graphic&gt;  is used for canvas graphics?</t>
+  </si>
+  <si>
+    <t>HTML is what type of Programming Language?</t>
+  </si>
+  <si>
+    <t>HTML uses User defined tags ?</t>
+  </si>
+  <si>
+    <t>The year in which HTML was first proposed 1990</t>
+  </si>
+  <si>
+    <t>Fundamental HTML Block is known as  HTML Tag</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;  bulleted list with numbers?</t>
+  </si>
+  <si>
+    <t>Tags and texts that are not directly displayed on the page are written in html section.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Drag and drop feature is supported in  HTML5</t>
+  </si>
+  <si>
+    <t>&lt;body&gt;  contains the meta information about the HTML page?</t>
+  </si>
+  <si>
+    <t>&lt;html&gt; root element of an HTML page?</t>
+  </si>
+  <si>
+    <t>HTML is a case sensitive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,10 +115,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF1D1E1F"/>
-      <name val="Open Sans"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="3"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,9 +166,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,178 +493,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0EA72A-597B-4240-BDEF-461CBB478F40}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H1:H10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.7109375" customWidth="1"/>
+    <col min="1" max="1" width="89.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>